<commit_message>
Updated version of FP calculation
</commit_message>
<xml_diff>
--- a/Software Requirements Specification/Use Cases/FP Calculation.xlsx
+++ b/Software Requirements Specification/Use Cases/FP Calculation.xlsx
@@ -5,21 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d070473\Git\eventlab-doc\Software Requirements Specification\Use Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d070473\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C5C80D6-A43A-41CA-AAF1-D363E28B5B01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDB017A-AEC1-4892-8272-0E9554B862B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{6D064F09-3B6D-4B42-AF0B-14BCEB8EDB3D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -30,51 +27,364 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="75">
+  <si>
+    <t>Function Points</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>FTR</t>
+  </si>
+  <si>
+    <t>Resulting Complexity</t>
+  </si>
+  <si>
+    <t>Number of</t>
+  </si>
+  <si>
+    <t>External Inputs</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Name, Email, Mesage, Submit</t>
+  </si>
+  <si>
+    <t>Contact Request</t>
+  </si>
+  <si>
+    <t>External Output</t>
+  </si>
+  <si>
+    <t>Confirmation</t>
+  </si>
+  <si>
+    <t>External Querie</t>
+  </si>
+  <si>
+    <t>Internal Logical Files</t>
+  </si>
+  <si>
+    <t>HTML, Controller, Email - Template</t>
+  </si>
+  <si>
+    <t>id, name, message, email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External Interface Files </t>
+  </si>
+  <si>
+    <t>Mail interface</t>
+  </si>
+  <si>
+    <t>Message, Password, Username, URL</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Name, Email, Password, Confirm Password, Submit</t>
+  </si>
+  <si>
+    <t>Create Account Request</t>
+  </si>
+  <si>
+    <t>User, Regestration Request</t>
+  </si>
+  <si>
+    <t>HTML, Controller, Confirm-HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 51
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High
+</t>
+  </si>
+  <si>
+    <t>Mail interface setup (Dovecot, Postfix, MySQL, Rspamd)</t>
+  </si>
+  <si>
+    <t>Title, Content, Submit, Create-btn</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Name, Inhalt, Datum</t>
+  </si>
+  <si>
+    <t>Journal, User, Views</t>
+  </si>
+  <si>
+    <t>id, name, owner, content, date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-
+</t>
+  </si>
+  <si>
+    <t>Name, Password</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show Feed
+</t>
+  </si>
+  <si>
+    <t>Controller, Home-html, Feed-html</t>
+  </si>
+  <si>
+    <t>Username, Password, email, regDate, verifiied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low
+</t>
+  </si>
+  <si>
+    <t>Email Interface</t>
+  </si>
+  <si>
+    <t>Estimation:</t>
+  </si>
+  <si>
+    <t>Upcomming Ucs</t>
+  </si>
+  <si>
+    <t>current password, old email, new email</t>
+  </si>
+  <si>
+    <t>Modal, Email</t>
+  </si>
+  <si>
+    <t>Delete-btn, Confirmation Dialog</t>
+  </si>
+  <si>
+    <t>OldPassword, NewPassword, repeat NewPassword</t>
+  </si>
+  <si>
+    <t>Modal</t>
+  </si>
+  <si>
+    <t>Various configs and commands</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>9.68</t>
+  </si>
+  <si>
+    <t>emailUUID, username, creationdate, verified, Email-Template</t>
+  </si>
+  <si>
+    <t>Change Email HTML, Controller</t>
+  </si>
+  <si>
+    <t>deleteUUID, username, creationdate, Email-Template</t>
+  </si>
+  <si>
+    <t>20.24</t>
+  </si>
+  <si>
+    <t>Email to old address, Email to new address, Modal</t>
+  </si>
+  <si>
+    <t>27.28</t>
+  </si>
   <si>
     <t>Use Case</t>
   </si>
   <si>
-    <t>Spent Time</t>
-  </si>
-  <si>
-    <t>Function Points</t>
+    <t>Spent Time (min)</t>
+  </si>
+  <si>
+    <t>Sum Spent Time / Sum Points</t>
+  </si>
+  <si>
+    <t>New Use Case</t>
+  </si>
+  <si>
+    <t>Calculated Time (min)</t>
   </si>
   <si>
     <t>CRUD Event</t>
   </si>
   <si>
-    <t>Crud Group</t>
+    <t>CRUD Group</t>
+  </si>
+  <si>
+    <t>Display Calendar</t>
   </si>
   <si>
     <t>Register</t>
   </si>
   <si>
-    <t>Display Calendar</t>
+    <t>Edit What-to-bring List</t>
+  </si>
+  <si>
+    <t>Manage Subscriptions</t>
+  </si>
+  <si>
+    <t>Reply to Events</t>
+  </si>
+  <si>
+    <t>Search Groups and Events</t>
+  </si>
+  <si>
+    <t>Send Chat Messages</t>
+  </si>
+  <si>
+    <t>Search Groups and events</t>
+  </si>
+  <si>
+    <t>Sum of old Ucs (min)</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="11">
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="-apple-system"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF6AA84F"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9B9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -82,18 +392,332 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="59">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9B9B"/>
+      <color rgb="FFFFB7B7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -119,45 +743,36 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.3803149606299209E-2"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.87753018372703417"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabellenblatt1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Function Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -180,30 +795,75 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$5</c:f>
+              <c:f>Tabellenblatt1!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7507</c:v>
+                  <c:v>2707</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6111</c:v>
+                  <c:v>2271</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4629</c:v>
+                  <c:v>2413</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7213</c:v>
+                  <c:v>1749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$5</c:f>
+              <c:f>Tabellenblatt1!$C$3:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -214,10 +874,10 @@
                   <c:v>128.26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.58</c:v>
+                  <c:v>47.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47.12</c:v>
+                  <c:v>36.58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -225,7 +885,86 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-495F-4862-AA26-8E635BC36F66}"/>
+              <c16:uniqueId val="{00000000-1CCA-49D4-A941-9525FD79B4F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabellenblatt1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Function Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabellenblatt1!$B$8:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1424.8704663212436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>580.82901554404145</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1865.2849740932643</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabellenblatt1!$C$8:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-1CCA-49D4-A941-9525FD79B4F7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -237,11 +976,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="500614616"/>
-        <c:axId val="500612976"/>
+        <c:axId val="366315992"/>
+        <c:axId val="366308776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="500614616"/>
+        <c:axId val="366315992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -298,12 +1037,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500612976"/>
+        <c:crossAx val="366308776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="500612976"/>
+        <c:axId val="366308776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -360,7 +1099,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500614616"/>
+        <c:crossAx val="366315992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -403,10 +1142,9 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -971,22 +1709,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:colOff>249116</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1673469</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>5862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Diagramm 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{887BB59D-B9AD-4D2F-A7E9-72FCCF4E87A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64D7A679-4BC3-45FA-A323-F7529B5418E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1005,56 +1743,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.075</cdr:x>
-      <cdr:y>0.21701</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.89167</cdr:x>
-      <cdr:y>0.8941</cdr:y>
-    </cdr:to>
-    <cdr:cxnSp macro="">
-      <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="3" name="Gerader Verbinder 2">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20DFCB97-753D-4A17-8EBF-A4F911F93F88}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvCxnSpPr/>
-      </cdr:nvCxnSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="342900" y="595313"/>
-          <a:ext cx="3733800" cy="1857375"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:style>
-        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </cdr:style>
-    </cdr:cxnSp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1353,80 +2041,1925 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD354419-8FAD-41E8-808D-71AC6D4EDED4}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
+      <c r="A2" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="39"/>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="35">
+        <v>2707</v>
+      </c>
+      <c r="C3" s="41">
+        <v>131.76</v>
+      </c>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:5" ht="15">
+      <c r="A4" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="35">
+        <v>2271</v>
+      </c>
+      <c r="C4" s="41">
+        <v>128.26</v>
+      </c>
+      <c r="E4" s="42"/>
+    </row>
+    <row r="5" spans="1:5" ht="15">
+      <c r="A5" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="35">
+        <v>2413</v>
+      </c>
+      <c r="C5" s="41">
+        <v>47.12</v>
+      </c>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="35">
+        <v>1749</v>
+      </c>
+      <c r="C6" s="41">
+        <v>36.58</v>
+      </c>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="45">
+        <f>1/0.0386*C8</f>
+        <v>1424.8704663212436</v>
+      </c>
+      <c r="C8" s="46">
+        <v>55</v>
+      </c>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="45">
+        <f t="shared" ref="B9:B12" si="0">1/0.0386*C9</f>
+        <v>580.82901554404145</v>
+      </c>
+      <c r="C9" s="41">
+        <v>22.42</v>
+      </c>
+      <c r="E9" s="42"/>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="45">
+        <f t="shared" si="0"/>
+        <v>1865.2849740932643</v>
+      </c>
+      <c r="C10" s="46">
+        <v>72</v>
+      </c>
+      <c r="E10" s="42"/>
+    </row>
+    <row r="11" spans="1:5" ht="15">
+      <c r="A11" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="45">
+        <f t="shared" si="0"/>
+        <v>550.25906735751289</v>
+      </c>
+      <c r="C11" s="46">
+        <v>21.24</v>
+      </c>
+      <c r="E11" s="42"/>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="A12" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="45">
+        <f t="shared" si="0"/>
+        <v>528.49740932642487</v>
+      </c>
+      <c r="C12" s="51">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E12" s="42"/>
+    </row>
+    <row r="13" spans="1:5" ht="12.75">
+      <c r="B13" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="A14" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="54">
+        <f>SUM(B3:B6)</f>
+        <v>9140</v>
+      </c>
+      <c r="C14" s="55">
+        <f>SUM(C3:C6)</f>
+        <v>343.71999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" thickBot="1">
+      <c r="A15" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="52">
+        <f>B14/C14</f>
+        <v>26.591411614104505</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="24"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A16" s="37"/>
+    </row>
+    <row r="17" spans="1:13" ht="15">
+      <c r="A17" s="36"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>7507</v>
-      </c>
-      <c r="C2">
-        <v>131.76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <f>5760+51+300</f>
-        <v>6111</v>
-      </c>
-      <c r="C3">
-        <v>128.26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <f>4320+9+300</f>
-        <v>4629</v>
-      </c>
-      <c r="C4">
-        <v>36.58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="G18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="12.75">
+      <c r="A19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <f>7200+13</f>
-        <v>7213</v>
-      </c>
-      <c r="C5">
-        <v>47.12</v>
-      </c>
+      <c r="B19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7">
+        <v>4</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="33"/>
+    </row>
+    <row r="20" spans="1:13" ht="12.75">
+      <c r="A20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="12.75">
+      <c r="A21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="12.75">
+      <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="7">
+        <v>3</v>
+      </c>
+      <c r="C22" s="7">
+        <v>4</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="7">
+        <v>2</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="12.75">
+      <c r="A23" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="14">
+        <v>1</v>
+      </c>
+      <c r="C23" s="14">
+        <v>4</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="14">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="12.75">
+      <c r="A26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="7">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="7">
+        <v>2</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="12.75">
+      <c r="A27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7">
+        <v>2</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="7">
+        <v>2</v>
+      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="12.75">
+      <c r="A28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="12.75">
+      <c r="A29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="7">
+        <v>3</v>
+      </c>
+      <c r="C29" s="7">
+        <v>7</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="7">
+        <v>2</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="19"/>
+      <c r="J29" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="12.75">
+      <c r="A30" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="14">
+        <v>4</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="14">
+        <v>1</v>
+      </c>
+      <c r="G30" s="15"/>
+      <c r="H30" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="12.75">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="12.75">
+      <c r="A33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="7">
+        <v>4</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="7">
+        <v>2</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="12.75">
+      <c r="A34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="7">
+        <v>1</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="12.75">
+      <c r="A35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="7">
+        <v>3</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="12.75">
+      <c r="A36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="7">
+        <v>5</v>
+      </c>
+      <c r="C36" s="7">
+        <v>5</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="7">
+        <v>3</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="12.75">
+      <c r="A37" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="14">
+        <v>0</v>
+      </c>
+      <c r="C37" s="14">
+        <v>0</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="14">
+        <v>0</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="12.75">
+      <c r="A38" s="20"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="12.75">
+      <c r="A40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="7">
+        <v>2</v>
+      </c>
+      <c r="D40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="12.75">
+      <c r="A41" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="7">
+        <v>4</v>
+      </c>
+      <c r="D41" s="7">
+        <v>2</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="12.75">
+      <c r="A42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="7">
+        <v>0</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J42" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="12.75">
+      <c r="A43" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="7">
+        <v>3</v>
+      </c>
+      <c r="C43" s="7">
+        <v>5</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="7">
+        <v>2</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="12.75">
+      <c r="A44" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="14">
+        <v>0</v>
+      </c>
+      <c r="C44" s="14">
+        <v>0</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="14">
+        <v>0</v>
+      </c>
+      <c r="G44" s="15"/>
+      <c r="H44" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J44" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="12.75">
+      <c r="A45" s="20"/>
+    </row>
+    <row r="46" spans="1:10" ht="12.75">
+      <c r="A46" s="26"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="27"/>
+    </row>
+    <row r="47" spans="1:10" ht="15">
+      <c r="A47" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="29"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A50" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="7">
+        <v>3</v>
+      </c>
+      <c r="D50" s="7">
+        <v>1</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0</v>
+      </c>
+      <c r="G50" s="8"/>
+      <c r="H50" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J50" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A51" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="7">
+        <v>2</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="7">
+        <v>1</v>
+      </c>
+      <c r="G51" s="8"/>
+      <c r="H51" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J51" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0</v>
+      </c>
+      <c r="G52" s="8"/>
+      <c r="H52" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J52" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A53" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="7">
+        <v>1</v>
+      </c>
+      <c r="C53" s="7">
+        <v>5</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="7">
+        <v>1</v>
+      </c>
+      <c r="G53" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A54" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="14">
+        <v>0</v>
+      </c>
+      <c r="C54" s="14">
+        <v>0</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="14">
+        <v>0</v>
+      </c>
+      <c r="G54" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="H54" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I54" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J54" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A56" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A57" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="7">
+        <v>3</v>
+      </c>
+      <c r="D57" s="7">
+        <v>1</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="7">
+        <v>0</v>
+      </c>
+      <c r="G57" s="8"/>
+      <c r="H57" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J57" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="7">
+        <v>3</v>
+      </c>
+      <c r="D58" s="7">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="7">
+        <v>3</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="H58" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J58" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0</v>
+      </c>
+      <c r="D59" s="7">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="7">
+        <v>0</v>
+      </c>
+      <c r="G59" s="8"/>
+      <c r="H59" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I59" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J59" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A60" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="7">
+        <v>2</v>
+      </c>
+      <c r="C60" s="7">
+        <v>5</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="7">
+        <v>2</v>
+      </c>
+      <c r="G60" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J60" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="14">
+        <v>1</v>
+      </c>
+      <c r="C61" s="14">
+        <v>0</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="14">
+        <v>1</v>
+      </c>
+      <c r="G61" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H61" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I61" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J61" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A63" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A64" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="7">
+        <v>2</v>
+      </c>
+      <c r="D64" s="7">
+        <v>1</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="7">
+        <v>1</v>
+      </c>
+      <c r="G64" s="8"/>
+      <c r="H64" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J64" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A65" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2</v>
+      </c>
+      <c r="D65" s="7">
+        <v>0</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="7">
+        <v>2</v>
+      </c>
+      <c r="G65" s="8"/>
+      <c r="H65" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J65" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A66" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0</v>
+      </c>
+      <c r="D66" s="7">
+        <v>0</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="7">
+        <v>0</v>
+      </c>
+      <c r="G66" s="8"/>
+      <c r="H66" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J66" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A67" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" s="7">
+        <v>1</v>
+      </c>
+      <c r="C67" s="7">
+        <v>3</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="7">
+        <v>1</v>
+      </c>
+      <c r="G67" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J67" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A68" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="14">
+        <v>1</v>
+      </c>
+      <c r="C68" s="14">
+        <v>0</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F68" s="14">
+        <v>1</v>
+      </c>
+      <c r="G68" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I68" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J68" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A70" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A71" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="7">
+        <v>3</v>
+      </c>
+      <c r="D71" s="7">
+        <v>1</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="7">
+        <v>0</v>
+      </c>
+      <c r="G71" s="8"/>
+      <c r="H71" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J71" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="7">
+        <v>2</v>
+      </c>
+      <c r="D72" s="7">
+        <v>0</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" s="7">
+        <v>1</v>
+      </c>
+      <c r="G72" s="8"/>
+      <c r="H72" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J72" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A73" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="7">
+        <v>0</v>
+      </c>
+      <c r="D73" s="7">
+        <v>0</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="7">
+        <v>0</v>
+      </c>
+      <c r="G73" s="8"/>
+      <c r="H73" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I73" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J73" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A74" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B74" s="7">
+        <v>1</v>
+      </c>
+      <c r="C74" s="7">
+        <v>5</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="7">
+        <v>1</v>
+      </c>
+      <c r="G74" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I74" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J74" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A75" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" s="14">
+        <v>0</v>
+      </c>
+      <c r="C75" s="14">
+        <v>0</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F75" s="14">
+        <v>0</v>
+      </c>
+      <c r="G75" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="H75" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I75" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J75" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A77" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A78" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="7">
+        <v>3</v>
+      </c>
+      <c r="D78" s="7">
+        <v>1</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="7">
+        <v>0</v>
+      </c>
+      <c r="G78" s="8"/>
+      <c r="H78" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J78" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A79" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="7">
+        <v>3</v>
+      </c>
+      <c r="D79" s="7">
+        <v>0</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="7">
+        <v>3</v>
+      </c>
+      <c r="G79" s="8"/>
+      <c r="H79" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J79" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A80" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="7">
+        <v>0</v>
+      </c>
+      <c r="D80" s="7">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="7">
+        <v>0</v>
+      </c>
+      <c r="G80" s="8"/>
+      <c r="H80" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I80" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J80" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A81" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B81" s="7">
+        <v>2</v>
+      </c>
+      <c r="C81" s="7">
+        <v>5</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="7">
+        <v>2</v>
+      </c>
+      <c r="G81" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I81" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J81" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A82" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" s="14">
+        <v>1</v>
+      </c>
+      <c r="C82" s="14">
+        <v>0</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F82" s="14">
+        <v>1</v>
+      </c>
+      <c r="G82" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H82" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I82" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J82" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="15.75" customHeight="1">
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+    </row>
+    <row r="96" spans="1:10" ht="15.75" customHeight="1">
+      <c r="D96" s="43"/>
+    </row>
+    <row r="97" spans="4:4" ht="15.75" customHeight="1">
+      <c r="D97" s="43"/>
+    </row>
+    <row r="98" spans="4:4" ht="15.75" customHeight="1">
+      <c r="D98" s="43"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G54" twoDigitTextYear="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>